<commit_message>
DATA: fix VE against hospitalisation for omicron (70+)
</commit_message>
<xml_diff>
--- a/inst/extdata/inputs/ve_estimates/ve_dat_round2_CD.xlsx
+++ b/inst/extdata/inputs/ve_estimates/ve_dat_round2_CD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\R\ainsliek\code\vacamole\inst\extdata\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\R\ainsliek\code\vacamole\inst\extdata\inputs\ve_estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C6C936-FAB4-4517-97AB-A4231EAFF47C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67138ACA-BE5F-41CF-A457-96F2359A6D3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1050" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{E62D7B7E-56A5-4CC4-8D62-76C0596AA6AC}"/>
+    <workbookView xWindow="1560" yWindow="2265" windowWidth="24780" windowHeight="11385" activeTab="3" xr2:uid="{E62D7B7E-56A5-4CC4-8D62-76C0596AA6AC}"/>
   </bookViews>
   <sheets>
     <sheet name="wildtype" sheetId="1" r:id="rId1"/>
@@ -25401,8 +25401,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H541"/>
   <sheetViews>
-    <sheetView topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="G155" sqref="G155:G226"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="M128" sqref="M128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38377,8 +38377,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H541"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H263" sqref="H263:H271"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="J389" sqref="J389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44744,10 +44744,10 @@
       </c>
       <c r="G261">
         <f t="shared" si="3"/>
-        <v>0.15322580645161282</v>
+        <v>0.35483870967741943</v>
       </c>
       <c r="H261">
-        <v>0.92400000000000004</v>
+        <v>0.82399999999999995</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
@@ -44771,10 +44771,10 @@
       </c>
       <c r="G262">
         <f t="shared" si="3"/>
-        <v>0.15322580645161282</v>
+        <v>0.35483870967741943</v>
       </c>
       <c r="H262">
-        <v>0.92400000000000004</v>
+        <v>0.82399999999999995</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
@@ -44987,10 +44987,10 @@
       </c>
       <c r="G270">
         <f t="shared" si="3"/>
-        <v>0.15322580645161282</v>
+        <v>0.35483870967741943</v>
       </c>
       <c r="H270">
-        <v>0.92400000000000004</v>
+        <v>0.82399999999999995</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
@@ -45014,10 +45014,10 @@
       </c>
       <c r="G271">
         <f t="shared" si="3"/>
-        <v>0.15322580645161282</v>
+        <v>0.35483870967741943</v>
       </c>
       <c r="H271">
-        <v>0.92400000000000004</v>
+        <v>0.82399999999999995</v>
       </c>
     </row>
     <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>